<commit_message>
[Update] Link entre songwheel et chart done ! Bug : Blood bugé dans la scène chart
Signed-off-by: Benoukat <ben.goze@gmail.com>
</commit_message>
<xml_diff>
--- a/Succes.xlsx
+++ b/Succes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>Plus que 999 heures de jeux</t>
   </si>
@@ -319,6 +319,54 @@
   </si>
   <si>
     <t>Obtenez 10 médailles de Quad</t>
+  </si>
+  <si>
+    <t>Clear 50 chansons différentes</t>
+  </si>
+  <si>
+    <t>Clear 600 chanson différentes</t>
+  </si>
+  <si>
+    <t>Clear 250 chansons différentes</t>
+  </si>
+  <si>
+    <t>Battez le boss 1</t>
+  </si>
+  <si>
+    <t>Battez le boss 2</t>
+  </si>
+  <si>
+    <t>Battez le boss 3</t>
+  </si>
+  <si>
+    <t>Battez le boss 4</t>
+  </si>
+  <si>
+    <t>Battez le boss 5</t>
+  </si>
+  <si>
+    <t>Battez le boss 6</t>
+  </si>
+  <si>
+    <t>Battez le boss 7</t>
+  </si>
+  <si>
+    <t>Battez le boss 8</t>
+  </si>
+  <si>
+    <t>Finissez Cublast</t>
+  </si>
+  <si>
+    <t>Obtenez toutes les médailles de bronze dans le mode Story</t>
+  </si>
+  <si>
+    <t>Obtenez toutes les médailles d'argent dans le mode Story</t>
+  </si>
+  <si>
+    <t>Obtenez toutes les médailles d'or dans le mode Story</t>
+  </si>
+  <si>
+    <t>Obtenez toutes les médailles de Quad dans le mode Story</t>
   </si>
 </sst>
 </file>
@@ -657,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1134,86 @@
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>